<commit_message>
C'etait encore tout cassé
grrr
</commit_message>
<xml_diff>
--- a/Data/BD Phantom Chief.xlsx
+++ b/Data/BD Phantom Chief.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89e17b0b139fae16/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rivar\Documents\Cours\MasterCamp\Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA69EE18-069B-4699-B1EB-9CB1B02FB6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CFE1D0-7925-4142-B144-594BB25F14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{847E3817-D3DD-4A02-80DE-8BE26FD902E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{847E3817-D3DD-4A02-80DE-8BE26FD902E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>Etape 1 : Dans un saladier verser la moitié de la farine, puis rajouter les oeufs un à un, rajouter ensuite un peu de lait puis de la farine puis à nouveau du lait et ainsi de suite. ; Etape 2 : Enfin rajouter l'huile et la bière. ; Etape 3 : Laisser reposer 1 heure, votre pâte est prête. ; Etape 4 : Cuire les crepes</t>
   </si>
   <si>
-    <t>10min,1,min,60min,30min</t>
-  </si>
-  <si>
     <t>louche,saladier,poêle à crêpes,cuillère en bois</t>
   </si>
   <si>
@@ -467,13 +464,16 @@
   </si>
   <si>
     <t>casserole,Mixeur,louche,cuillère en bois</t>
+  </si>
+  <si>
+    <t>10min,1min,60min,30min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -857,25 +857,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F8CDD6-A075-4310-A7A1-DECAE5545030}">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="71.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="219.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="219.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="76.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="76.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="11.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,7 +907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -971,7 +971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1020,10 +1020,10 @@
         <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>24</v>
@@ -1032,30 +1032,30 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="11.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>24</v>
@@ -1064,30 +1064,30 @@
         <v>2</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="11.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>16</v>
@@ -1099,27 +1099,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>24</v>
@@ -1131,27 +1131,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
@@ -1163,27 +1163,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>24</v>
@@ -1195,27 +1195,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>24</v>
@@ -1227,30 +1227,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="I12" s="2">
         <v>4</v>
@@ -1259,27 +1259,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
@@ -1291,27 +1291,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>24</v>
@@ -1320,30 +1320,30 @@
         <v>4</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="11.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>24</v>
@@ -1352,30 +1352,30 @@
         <v>2</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="11.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>16</v>
@@ -1384,33 +1384,33 @@
         <v>4</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="11.25" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="2">
         <v>6</v>
@@ -1419,27 +1419,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="18" spans="1:10" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>24</v>
@@ -1451,27 +1451,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="19" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>24</v>
@@ -1483,27 +1483,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>16</v>
@@ -1515,27 +1515,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="11.25" customHeight="1">
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>24</v>
@@ -1547,27 +1547,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" ht="11.25">
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>24</v>
@@ -1579,82 +1579,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="11.25"/>
-    <row r="24" spans="1:10" ht="11.25"/>
-    <row r="25" spans="1:10" ht="11.25"/>
-    <row r="26" spans="1:10" ht="11.25"/>
-    <row r="27" spans="1:10" ht="11.25"/>
-    <row r="28" spans="1:10" ht="11.25"/>
-    <row r="29" spans="1:10" ht="11.25"/>
-    <row r="30" spans="1:10" ht="11.25"/>
-    <row r="31" spans="1:10" ht="11.25"/>
-    <row r="32" spans="1:10" ht="11.25"/>
-    <row r="33" ht="11.25"/>
-    <row r="34" ht="11.25"/>
-    <row r="35" ht="11.25"/>
-    <row r="36" ht="11.25"/>
-    <row r="37" ht="11.25"/>
-    <row r="38" ht="11.25"/>
-    <row r="39" ht="11.25"/>
-    <row r="40" ht="11.25"/>
-    <row r="41" ht="11.25"/>
-    <row r="42" ht="11.25"/>
-    <row r="43" ht="11.25"/>
-    <row r="44" ht="11.25"/>
-    <row r="45" ht="11.25"/>
-    <row r="46" ht="11.25"/>
-    <row r="47" ht="11.25"/>
-    <row r="48" ht="11.25"/>
-    <row r="49" ht="11.25"/>
-    <row r="50" ht="11.25"/>
-    <row r="51" ht="11.25"/>
-    <row r="52" ht="11.25"/>
-    <row r="53" ht="11.25"/>
-    <row r="54" ht="11.25"/>
-    <row r="55" ht="11.25"/>
-    <row r="56" ht="11.25"/>
-    <row r="57" ht="11.25"/>
-    <row r="58" ht="11.25"/>
-    <row r="59" ht="11.25"/>
-    <row r="60" ht="11.25"/>
-    <row r="61" ht="11.25"/>
-    <row r="62" ht="11.25"/>
-    <row r="63" ht="11.25"/>
-    <row r="64" ht="11.25"/>
-    <row r="65" ht="11.25"/>
-    <row r="66" ht="11.25"/>
-    <row r="67" ht="11.25"/>
-    <row r="68" ht="11.25"/>
-    <row r="69" ht="11.25"/>
-    <row r="70" ht="11.25"/>
-    <row r="71" ht="11.25"/>
-    <row r="72" ht="11.25"/>
-    <row r="73" ht="11.25"/>
-    <row r="74" ht="11.25"/>
-    <row r="75" ht="11.25"/>
-    <row r="76" ht="11.25"/>
-    <row r="77" ht="11.25"/>
-    <row r="78" ht="11.25"/>
-    <row r="79" ht="11.25"/>
-    <row r="80" ht="11.25"/>
-    <row r="81" ht="11.25"/>
-    <row r="82" ht="11.25"/>
-    <row r="83" ht="11.25"/>
-    <row r="84" ht="11.25"/>
-    <row r="85" ht="11.25"/>
-    <row r="86" ht="11.25"/>
-    <row r="87" ht="11.25"/>
-    <row r="88" ht="11.25"/>
-    <row r="89" ht="11.25"/>
-    <row r="90" ht="11.25"/>
-    <row r="91" ht="11.25"/>
-    <row r="92" ht="11.25"/>
-    <row r="93" ht="11.25"/>
-    <row r="94" ht="11.25"/>
-    <row r="95" ht="11.25"/>
-    <row r="96" ht="11.25"/>
-    <row r="97" ht="11.25"/>
-    <row r="98" ht="11.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>